<commit_message>
Changed the input file URL
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://opteamix-my.sharepoint.com/personal/ssatish_opteamix_com/Documents/Documents/UiPath/RPA Challenge Assignment 3/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F7422611-2731-4A9E-80F4-5066F37D7A99}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD4D86A1-4169-481B-844F-E24DDEC0FEF5}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -165,9 +165,6 @@
     <t>InputFile</t>
   </si>
   <si>
-    <t>C:\Users\SSatish\OneDrive - Opteamix LLC\Documents\UiPath\RPA Challenge Assignment 3\Data\Input\challenge.xlsx</t>
-  </si>
-  <si>
     <t>InputSheet</t>
   </si>
   <si>
@@ -178,6 +175,9 @@
   </si>
   <si>
     <t>https://www.rpachallenge.com/</t>
+  </si>
+  <si>
+    <t>Data\Input\challenge.xlsx</t>
   </si>
 </sst>
 </file>
@@ -229,7 +229,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -239,7 +239,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -255,6 +254,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -556,8 +559,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
@@ -640,23 +643,23 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1">
       <c r="A8" t="s">
+        <v>46</v>
+      </c>
+      <c r="B8" t="s">
         <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1">
       <c r="A9" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
         <v>49</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1659,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Z988"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>

</xml_diff>